<commit_message>
add g1 moderators doc
</commit_message>
<xml_diff>
--- a/docs/g1-moderators.xlsx
+++ b/docs/g1-moderators.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Research\FSW\Research_data\JG\SanneG\ICITOP IPD_MA\icitop\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677620EC-0E88-4555-9C56-4FC2E29E38E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6510"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$50</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="27">
   <si>
     <t>generation</t>
   </si>
@@ -65,19 +69,52 @@
     <t>age</t>
   </si>
   <si>
-    <t>g2</t>
-  </si>
-  <si>
     <t>par</t>
   </si>
   <si>
     <t>name_construct</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>rst</t>
+  </si>
+  <si>
+    <t>rso</t>
+  </si>
+  <si>
+    <t>inv</t>
+  </si>
+  <si>
+    <t>cst</t>
+  </si>
+  <si>
+    <t>ris</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g2 </t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g1 </t>
+  </si>
+  <si>
+    <t>eth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,11 +425,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -405,7 +442,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -416,7 +453,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -424,7 +464,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -432,10 +475,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -443,10 +486,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -454,10 +497,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -465,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -476,7 +519,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -484,7 +530,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -495,7 +541,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -506,7 +552,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -514,7 +563,10 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -522,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -533,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -541,13 +593,457 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
         <v>12</v>
       </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C50" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add empty target rows
</commit_message>
<xml_diff>
--- a/docs/g1-moderators.xlsx
+++ b/docs/g1-moderators.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Research\FSW\Research_data\JG\SanneG\ICITOP IPD_MA\icitop\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677620EC-0E88-4555-9C56-4FC2E29E38E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3056AC8A-B1A0-4D74-88EE-EF8D817DC758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$75</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="28">
   <si>
     <t>generation</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>eth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">car </t>
   </si>
 </sst>
 </file>
@@ -426,18 +429,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -459,7 +462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -470,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -481,7 +484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -492,7 +495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -503,7 +506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -514,7 +517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -525,7 +528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -536,7 +539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -547,7 +550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -558,7 +561,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -569,7 +572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -580,7 +583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -591,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -602,7 +605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -613,7 +616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -624,7 +627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -635,7 +638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -646,7 +649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -657,7 +660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -668,7 +671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -679,7 +682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -690,7 +693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -701,7 +704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -712,7 +715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -723,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -734,7 +737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -745,7 +748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -756,7 +759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -767,7 +770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -778,7 +781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -789,7 +792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -800,7 +803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -811,7 +814,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -822,7 +825,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -833,7 +836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -844,7 +847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -855,7 +858,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -866,7 +869,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -877,7 +880,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -888,7 +891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -899,7 +902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -910,7 +913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -921,7 +924,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -932,7 +935,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -943,7 +946,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -954,7 +957,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -965,7 +968,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -976,7 +979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -987,7 +990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>22</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -1042,8 +1045,168 @@
         <v>23</v>
       </c>
     </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C50" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C75" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>